<commit_message>
update for trim header of excel test data
update for trim header of excel test data
</commit_message>
<xml_diff>
--- a/test/_qaf_loadfeature/testdata/testdata.xlsx
+++ b/test/_qaf_loadfeature/testdata/testdata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\playwright-bdd\test\_qaf_loadfeature\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2070812\OneDrive - Cognizant\Documents\GitHub\playwright-bdd\test\_qaf_loadfeature\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{146570EE-AD2E-498F-BB8D-EB2DB8480C30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A7075DC-7B25-434F-B683-A59B53F5B783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="1520" windowWidth="21600" windowHeight="12760" tabRatio="664" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20340" yWindow="-9630" windowWidth="28800" windowHeight="15370" tabRatio="664" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FirstSheet" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="SheetWithoutHeader" sheetId="3" r:id="rId7"/>
     <sheet name="integration_DataTable1" sheetId="8" r:id="rId8"/>
     <sheet name="integration_DataTable2" sheetId="9" r:id="rId9"/>
+    <sheet name="integration_DataTable3" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="82">
   <si>
     <t>Id</t>
   </si>
@@ -281,6 +282,12 @@
   </si>
   <si>
     <t>end</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     end   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    start    </t>
   </si>
 </sst>
 </file>
@@ -291,20 +298,20 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -331,11 +338,11 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="58" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -614,10 +621,10 @@
       <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11.08203125" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="8.4609375" customWidth="1"/>
-    <col min="7" max="7" width="17.15234375" customWidth="1"/>
+    <col min="1" max="1" width="8.5" customWidth="1"/>
+    <col min="7" max="7" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -743,6 +750,53 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C4DCD28-98CB-46E0-BB8E-A2FB6BD23AE3}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.5"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -752,10 +806,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11.08203125" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="8.4609375" customWidth="1"/>
-    <col min="7" max="7" width="17.15234375" customWidth="1"/>
+    <col min="1" max="1" width="8.5" customWidth="1"/>
+    <col min="7" max="7" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -892,11 +946,11 @@
       <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11.08203125" defaultRowHeight="15.5"/>
   <cols>
-    <col min="9" max="9" width="17.69140625" customWidth="1"/>
-    <col min="10" max="10" width="19.15234375" customWidth="1"/>
-    <col min="15" max="15" width="13.84375" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" customWidth="1"/>
+    <col min="10" max="10" width="19.1640625" customWidth="1"/>
+    <col min="15" max="15" width="13.83203125" customWidth="1"/>
     <col min="16" max="16" width="24" customWidth="1"/>
     <col min="19" max="19" width="18" customWidth="1"/>
   </cols>
@@ -1565,8 +1619,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="13.765625" customWidth="1"/>
-    <col min="2" max="2" width="34.15234375" customWidth="1"/>
+    <col min="1" max="1" width="13.75" customWidth="1"/>
+    <col min="2" max="2" width="34.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1622,12 +1676,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.5"/>
   <cols>
-    <col min="2" max="2" width="13.765625" customWidth="1"/>
-    <col min="3" max="3" width="34.15234375" customWidth="1"/>
-    <col min="4" max="4" width="7.3828125" customWidth="1"/>
-    <col min="8" max="8" width="20.53515625" customWidth="1"/>
-    <col min="9" max="9" width="24.84375" customWidth="1"/>
-    <col min="10" max="10" width="11.765625" customWidth="1"/>
+    <col min="2" max="2" width="13.75" customWidth="1"/>
+    <col min="3" max="3" width="34.1640625" customWidth="1"/>
+    <col min="4" max="4" width="7.4140625" customWidth="1"/>
+    <col min="8" max="8" width="20.5" customWidth="1"/>
+    <col min="9" max="9" width="24.83203125" customWidth="1"/>
+    <col min="10" max="10" width="11.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:11">
@@ -1819,14 +1873,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="13.765625" customWidth="1"/>
-    <col min="2" max="2" width="34.15234375" customWidth="1"/>
+    <col min="1" max="1" width="13.75" customWidth="1"/>
+    <col min="2" max="2" width="34.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1876,10 +1930,10 @@
       <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11.08203125" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="8.4609375" customWidth="1"/>
-    <col min="7" max="7" width="17.15234375" customWidth="1"/>
+    <col min="1" max="1" width="8.5" customWidth="1"/>
+    <col min="7" max="7" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1993,10 +2047,10 @@
       <selection activeCell="I9" sqref="I9:J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.921875" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="15.5"/>
   <cols>
-    <col min="8" max="8" width="5.84375" customWidth="1"/>
-    <col min="10" max="10" width="9.69140625" customWidth="1"/>
+    <col min="8" max="8" width="5.83203125" customWidth="1"/>
+    <col min="10" max="10" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="9" spans="8:12">
@@ -2054,7 +2108,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04726056-9C67-4238-8490-A15181FC45BE}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5"/>
   <sheetData>

</xml_diff>